<commit_message>
final working flows used to record demos
</commit_message>
<xml_diff>
--- a/schemas/WorkdayToMaximoMappings.xlsx
+++ b/schemas/WorkdayToMaximoMappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos.ferreira1ibm.com/ws/workday/maximo-workday/schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B77A36C-FFC4-6048-AEAC-4E4B60DD7A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879C1130-B6DB-EB45-864A-12ADB59BA72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13700" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{90F71F93-E3B8-BA46-A8B2-D88EA043161D}"/>
+    <workbookView xWindow="13700" yWindow="460" windowWidth="35840" windowHeight="20600" xr2:uid="{90F71F93-E3B8-BA46-A8B2-D88EA043161D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="233">
   <si>
     <t>Workday</t>
   </si>
@@ -659,9 +659,6 @@
     <t>required</t>
   </si>
   <si>
-    <t>Standard Rate</t>
-  </si>
-  <si>
     <t>Missing in REST Skills Report.json</t>
   </si>
   <si>
@@ -716,10 +713,25 @@
     <t>maximo_workday_intial_setup_crafts</t>
   </si>
   <si>
-    <t>equals"Report_Entry": [{"JobProfileName": "Electrician Apprentice"},</t>
-  </si>
-  <si>
     <t>maximo_workday_get_integration_events</t>
+  </si>
+  <si>
+    <t>Update or Create Craft</t>
+  </si>
+  <si>
+    <t>Job_profile_name</t>
+  </si>
+  <si>
+    <t>Job_profile_ID</t>
+  </si>
+  <si>
+    <t>CRAFTID</t>
+  </si>
+  <si>
+    <t>Manually set in flow.</t>
+  </si>
+  <si>
+    <t>Job_profile_name from Crafts "Report_Entry": [{"JobProfileName": "Electrician Apprentice"},</t>
   </si>
 </sst>
 </file>
@@ -1125,9 +1137,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C639F693-642A-4D47-924F-E0AED835A2B9}">
   <dimension ref="A1:N183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M79" sqref="M79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1142,29 +1154,29 @@
     <col min="9" max="9" width="19.1640625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="50.1640625" customWidth="1"/>
+    <col min="12" max="12" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" t="s">
         <v>219</v>
       </c>
-      <c r="C1" t="s">
-        <v>220</v>
-      </c>
       <c r="G1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" t="s">
         <v>219</v>
-      </c>
-      <c r="H1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1176,13 +1188,13 @@
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>182</v>
@@ -1220,7 +1232,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>187</v>
@@ -1244,7 +1256,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>188</v>
@@ -1274,10 +1286,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>189</v>
@@ -1872,68 +1884,74 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
       <c r="M75" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I76" t="s">
         <v>207</v>
       </c>
       <c r="J76" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K76" s="7"/>
       <c r="L76" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M76" s="7"/>
       <c r="N76" s="7"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H77" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I77" t="s">
         <v>207</v>
       </c>
       <c r="J77" s="7"/>
       <c r="K77" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L77" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="M77" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="M77" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="N77" s="7"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H78" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I78" t="s">
         <v>207</v>
       </c>
       <c r="J78" s="7"/>
       <c r="K78" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L78" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C79" t="s">
+        <v>228</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>197</v>
@@ -1948,16 +1966,19 @@
         <v>15</v>
       </c>
       <c r="K79" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L79" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="M79" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>231</v>
+      </c>
       <c r="H80" t="s">
         <v>80</v>
       </c>
@@ -1969,19 +1990,25 @@
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>229</v>
+      </c>
       <c r="H81" s="7" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
+      <c r="L81" t="s">
+        <v>229</v>
+      </c>
       <c r="M81" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>190</v>

</xml_diff>